<commit_message>
working parcel builder ipynb
</commit_message>
<xml_diff>
--- a/layer-building/parcel_data/ppa_pcl_data_dict.xlsx
+++ b/layer-building/parcel_data/ppa_pcl_data_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\layer-building\parcel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5E73F49D-B129-4C7E-8612-116E76B79FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAB2102-8FBC-49BD-8B8C-88EF960D7EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFBDBC86-3DFB-406E-A9A8-2287EA45AF17}"/>
   </bookViews>
@@ -22,7 +22,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">pcl_polys!$A$1:$E$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">placetype_consolidation!$A$1:$B$49</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1134,7 +1147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1273,6 +1286,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1616,11 +1636,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1999,7 +2020,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2142,20 +2163,20 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" s="2" customFormat="1">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>365</v>
       </c>
     </row>

</xml_diff>